<commit_message>
visualisation version presque finale
</commit_message>
<xml_diff>
--- a/src/LivinParis/data/metro/MetroParis.xlsx
+++ b/src/LivinParis/data/metro/MetroParis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliot\RiderProjects\LivinParis\src\LivinParis\data\metro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4434DA1-AC2E-4DD3-9FB6-57A6DA76365D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234C38F-B07B-4478-B401-03E9FC313200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6A7959BE-A0B4-4EB6-8342-15F77AC26B90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6A7959BE-A0B4-4EB6-8342-15F77AC26B90}"/>
   </bookViews>
   <sheets>
     <sheet name="stations" sheetId="1" r:id="rId1"/>
@@ -1630,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6549EE12-F9D9-4064-922E-DFCA0A3CB738}">
   <dimension ref="A1:G332"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C176" sqref="C176:C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9342,8 +9342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CFEF04-CB9F-4D0E-AA44-E5CDB48F03B4}">
   <dimension ref="A1:G333"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="F259" sqref="F259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12448,9 +12448,7 @@
       <c r="C180" t="s">
         <v>170</v>
       </c>
-      <c r="D180" s="1">
-        <v>177</v>
-      </c>
+      <c r="D180" s="1"/>
       <c r="E180" s="1">
         <v>173</v>
       </c>
@@ -13837,7 +13835,7 @@
         <v>10</v>
       </c>
       <c r="E261">
-        <v>300</v>
+        <v>330</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -13850,9 +13848,7 @@
       <c r="C262">
         <v>10</v>
       </c>
-      <c r="D262" s="1">
-        <v>259</v>
-      </c>
+      <c r="D262" s="1"/>
       <c r="E262" s="1">
         <v>252</v>
       </c>
@@ -15143,7 +15139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36DDB5DC-C1CD-4F1F-BA58-6481AB17756E}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>